<commit_message>
Updated text to reflect use of Folium for mapping
</commit_message>
<xml_diff>
--- a/data/distancetableFL.xlsx
+++ b/data/distancetableFL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fxkelly/notebooks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0BDA66-211A-CD41-9A10-6109891EDCD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD8999D-9498-6940-82A5-7A7282393E92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9540" yWindow="8780" windowWidth="27240" windowHeight="16040" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6480" yWindow="3520" windowWidth="27240" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="8" r:id="rId1"/>
@@ -778,15 +778,9 @@
     <t>terminaldata</t>
   </si>
   <si>
-    <t>M x 8</t>
-  </si>
-  <si>
     <t>generated using openrouteservice.org</t>
   </si>
   <si>
-    <t>data for terminals: name, latitude, longitude, color (for map), extratime (trip-time beyond calculated for route: load, discharge, any delays), supply cost, maximum gal/month that can be supplied from a terminal (to all the stations it supplies), minimum offtake</t>
-  </si>
-  <si>
     <t>tab</t>
   </si>
   <si>
@@ -845,6 +839,12 @@
   </si>
   <si>
     <t>3300 NW 87th Avenue Doral, FL 33172</t>
+  </si>
+  <si>
+    <t>M x 10</t>
+  </si>
+  <si>
+    <t>data for terminals: name, number, latitude, longitude, color (for map)...hexcode and name (latter required for folium), extratime (trip-time beyond calculated for route: load, discharge, any delays), supply cost, maximum gal/month that can be supplied from a terminal (to all the stations it supplies), minimum offtake</t>
   </si>
 </sst>
 </file>
@@ -1689,10 +1689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{923E65F7-833F-FD4E-99C3-4FF1026DDA2F}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21:F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1704,13 +1704,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C1" t="s">
         <v>253</v>
-      </c>
-      <c r="B1" t="s">
-        <v>254</v>
-      </c>
-      <c r="C1" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1724,7 +1724,7 @@
         <v>232</v>
       </c>
       <c r="D2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1738,7 +1738,7 @@
         <v>233</v>
       </c>
       <c r="D3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1760,10 +1760,10 @@
         <v>249</v>
       </c>
       <c r="B5" t="s">
-        <v>250</v>
+        <v>271</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1788,46 +1788,14 @@
       </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E17" s="1">
-        <v>33.32</v>
-      </c>
-      <c r="F17" s="1">
-        <v>244.06</v>
-      </c>
-      <c r="G17" s="1">
-        <v>277.33999999999997</v>
-      </c>
-      <c r="H17" s="1">
-        <v>273.82</v>
-      </c>
-      <c r="I17" s="1">
-        <v>216.8</v>
-      </c>
-      <c r="J17" s="1">
-        <v>231.78</v>
-      </c>
-      <c r="K17" s="1">
-        <v>355.26</v>
-      </c>
-      <c r="L17" s="1">
-        <v>359.01</v>
-      </c>
-    </row>
-    <row r="19" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E19">
-        <v>-80.315368000000007</v>
-      </c>
-      <c r="F19">
-        <v>25.764150000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E21">
-        <v>-80.372941999999995</v>
-      </c>
-      <c r="F21">
-        <v>25.583760999999999</v>
-      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1838,9 +1806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I213"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:R5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -14223,7 +14189,7 @@
   <dimension ref="A1:B213"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15941,14 +15907,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A67BAB-A16B-0946-A919-B102AD1C268C}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -15956,31 +15920,31 @@
         <v>240</v>
       </c>
       <c r="C1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" t="s">
         <v>219</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>220</v>
       </c>
-      <c r="E1" t="s">
-        <v>263</v>
-      </c>
       <c r="F1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H1" t="s">
         <v>239</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>227</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>241</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>242</v>
-      </c>
-      <c r="J1" t="s">
-        <v>262</v>
-      </c>
-      <c r="K1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -15991,31 +15955,31 @@
         <v>216</v>
       </c>
       <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>-80.131586999999996</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>26.089092999999998</v>
       </c>
-      <c r="E2" t="s">
-        <v>256</v>
-      </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>254</v>
+      </c>
+      <c r="G2" t="s">
+        <v>262</v>
+      </c>
+      <c r="H2">
         <v>60</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>0</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>7000000</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>500000</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -16026,31 +15990,31 @@
         <v>0</v>
       </c>
       <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>-82.557091</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>27.637357999999999</v>
       </c>
-      <c r="E3" t="s">
-        <v>257</v>
-      </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>255</v>
+      </c>
+      <c r="G3" t="s">
+        <v>265</v>
+      </c>
+      <c r="H3">
         <v>60</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>0</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>7000000</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>500000</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -16061,31 +16025,31 @@
         <v>1</v>
       </c>
       <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
         <v>-82.548224000000005</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>27.858483</v>
       </c>
-      <c r="E4" t="s">
-        <v>258</v>
-      </c>
-      <c r="F4">
+      <c r="F4" t="s">
+        <v>256</v>
+      </c>
+      <c r="G4" t="s">
+        <v>264</v>
+      </c>
+      <c r="H4">
         <v>60</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>0</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>7000000</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>500000</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
-      <c r="K4" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -16096,31 +16060,31 @@
         <v>2</v>
       </c>
       <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
         <v>-82.441068000000001</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>27.951598000000001</v>
       </c>
-      <c r="E5" t="s">
-        <v>259</v>
-      </c>
-      <c r="F5">
+      <c r="F5" t="s">
+        <v>257</v>
+      </c>
+      <c r="G5" t="s">
+        <v>269</v>
+      </c>
+      <c r="H5">
         <v>60</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>0</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>7000000</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>500000</v>
-      </c>
-      <c r="J5">
-        <v>3</v>
-      </c>
-      <c r="K5" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -16131,31 +16095,31 @@
         <v>3</v>
       </c>
       <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
         <v>-80.605376000000007</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>28.404253000000001</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>223</v>
       </c>
-      <c r="F6">
+      <c r="G6" t="s">
+        <v>263</v>
+      </c>
+      <c r="H6">
         <v>60</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>0</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>7000000</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>500000</v>
-      </c>
-      <c r="J6">
-        <v>4</v>
-      </c>
-      <c r="K6" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -16166,31 +16130,31 @@
         <v>4</v>
       </c>
       <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
         <v>-81.373255</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>28.421876999999999</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>222</v>
       </c>
-      <c r="F7">
+      <c r="G7" t="s">
+        <v>266</v>
+      </c>
+      <c r="H7">
         <v>60</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>0</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>7000000</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>500000</v>
-      </c>
-      <c r="J7">
-        <v>5</v>
-      </c>
-      <c r="K7" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -16201,31 +16165,31 @@
         <v>217</v>
       </c>
       <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
         <v>-81.626013</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>30.360426</v>
       </c>
-      <c r="E8" t="s">
-        <v>261</v>
-      </c>
-      <c r="F8">
+      <c r="F8" t="s">
+        <v>259</v>
+      </c>
+      <c r="G8" t="s">
+        <v>267</v>
+      </c>
+      <c r="H8">
         <v>60</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>0</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>7000000</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>500000</v>
-      </c>
-      <c r="J8">
-        <v>6</v>
-      </c>
-      <c r="K8" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -16236,31 +16200,31 @@
         <v>218</v>
       </c>
       <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
         <v>-81.609499999999997</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>30.417065999999998</v>
       </c>
-      <c r="E9" t="s">
-        <v>260</v>
-      </c>
-      <c r="F9">
+      <c r="F9" t="s">
+        <v>258</v>
+      </c>
+      <c r="G9" t="s">
+        <v>268</v>
+      </c>
+      <c r="H9">
         <v>60</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>0</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>7000000</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>500000</v>
-      </c>
-      <c r="J9">
-        <v>7</v>
-      </c>
-      <c r="K9" t="s">
-        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -16335,7 +16299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E96A2560-92D6-3944-89BE-FE247940F8DA}">
   <dimension ref="A1:D213"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -16416,7 +16380,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C6">
         <v>-80.337776000000005</v>

</xml_diff>